<commit_message>
update schedule and 解答
</commit_message>
<xml_diff>
--- a/schedule/schedule.xlsx
+++ b/schedule/schedule.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F455DD3E-A3B4-4A51-A8FF-EFCEF32DA3CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>任务</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,58 +72,68 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Done（但是内部类有点乱）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Java第8章面向对象编程
+2.Activity的使用(跳转startActivity，有返回结果的跳转startActivityForResult，生命周期，启动模式等)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一行代码的第二章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Java第9章异常处理
+2.BroadcastReceiver(自定义广播，系统广播，有序广播)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一行代码的第五章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Java第10章线程
+2.RecyclerView的用法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一行代码第三章(3.6), 内容不多，可以上网看看别人如何使用RecyclerView或者巩固一下前面的内容。现在基本不用ListView了，都是使用RecyclerView</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java完成了，但是android的还剩一些没看完。（这两天会完成的）    (Done 4.15)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>今天没完成（反省…）4.16           大体看了下要求的内容，首先关于线程的问题，感觉只是看了，了解了下基本的一些概念，不知道怎么去用==然后Android的recyclerview用法，感觉功能蛮多的啊，开始出现的适配器啥的，网上一搜，就是啪一堆的，所以需要掌握哪些，只要会用这个组件就好了（反正看的是云里雾里的）？（4.17）                        重新看了第一行代码的内容，算是了解基本的用法，笔记记在本子上，没有弄到word里面上传                    （4.18）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.Java第7章接口和内部类
 2.写一个登录界面(界面如:登录界面.png)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Done（但是内部类有点乱）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.Java第8章面向对象编程
-2.Activity的使用(跳转startActivity，有返回结果的跳转startActivityForResult，生命周期，启动模式等)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一行代码的第二章</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.Java第9章异常处理
-2.BroadcastReceiver(自定义广播，系统广播，有序广播)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一行代码的第五章</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.Java第10章线程
-2.RecyclerView的用法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一行代码第三章(3.6), 内容不多，可以上网看看别人如何使用RecyclerView或者巩固一下前面的内容。现在基本不用ListView了，都是使用RecyclerView</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Java完成了，但是android的还剩一些没看完。（这两天会完成的）    (Done 4.15)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>今天没完成（反省…）4.16           大体看了下要求的内容，首先关于线程的问题，感觉只是看了，了解了下基本的一些概念，不知道怎么去用==然后Android的recyclerview用法，感觉功能蛮多的啊，开始出现的适配器啥的，网上一搜，就是啪一堆的，所以需要掌握哪些，只要会用这个组件就好了（反正看的是云里雾里的）？（4.17）                        重新看了第一行代码的内容，算是了解基本的用法，笔记记在本子上，没有弄到word里面上传                    （4.18）</t>
+    <t>1.Java另一本书的第10章集合类
+2.使用RecyclerView写一个仿微信列表(界面如:列表.jpg)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看另一本Java从入门到精通。
+界面只要关注红色框框部分，就是只关注列表的实现，另外有个黑框圈起来的可以忽略那个部分，也就是每个item大概由四个部分组成(给两天时间)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,26 +328,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -371,23 +363,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -563,23 +538,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="40.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.875" customWidth="1"/>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -596,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="161" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -613,7 +588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="138" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -630,9 +605,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="138" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B4" s="7">
         <v>43201</v>
@@ -644,12 +619,12 @@
         <v>11</v>
       </c>
       <c r="E4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="138" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="B5" s="7">
         <v>43202</v>
@@ -658,15 +633,15 @@
         <v>43202</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="9" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="92" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="B6" s="7">
         <v>43203</v>
@@ -675,166 +650,174 @@
         <v>43205</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="207" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="B7" s="7">
         <v>43205</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="7">
+        <v>43208</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="23" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="7">
+        <v>43210</v>
+      </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -847,12 +830,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -860,12 +843,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update schecule and 解答
</commit_message>
<xml_diff>
--- a/schedule/schedule.xlsx
+++ b/schedule/schedule.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1A624FAD-6B52-4023-8AE8-D36EC3652683}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>任务</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,24 +120,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>看另一本Java从入门到精通。
+界面只要关注红色框框部分，就是只关注列表的实现，另外有个黑框圈起来的可以忽略那个部分，也就是每个item大概由四个部分组成(给两天时间)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android部分已经完成（后面加了分割线，还给图片加了边框）         Java就是了解有哪些集合类，下面有哪些接口，接口下面有哪些方法    （4.20）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1.Java另一本书的第10章集合类
 2.使用RecyclerView写一个仿微信列表(界面如:列表.jpg)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>看另一本Java从入门到精通。
-界面只要关注红色框框部分，就是只关注列表的实现，另外有个黑框圈起来的可以忽略那个部分，也就是每个item大概由四个部分组成(给两天时间)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android部分已经完成（后面加了分割线，还给图片加了边框）         Java就是了解有哪些集合类，下面有哪些接口，接口下面有哪些方法    （4.20）</t>
+    <t>第一行代码的第10章
+要弄清楚什么时候用startService,什么使用bindService。bindService还是比较复杂的，所以要注意记录步骤，否则又乱了。
+这章就有很多跟线程有关的东西了。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.Java另一本书的第12章输入/输出
+2.Handler, AsyncTask的使用
+3.Service的用法(startService和bindService,生命周期)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -300,7 +311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,26 +344,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,23 +379,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -577,23 +554,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="40.90625" customWidth="1"/>
-    <col min="2" max="2" width="33.90625" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" customWidth="1"/>
-    <col min="4" max="4" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.6328125" customWidth="1"/>
+    <col min="1" max="1" width="40.875" customWidth="1"/>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="22.75" customWidth="1"/>
+    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -610,7 +587,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="161" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -627,7 +604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="138" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -644,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="138" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -661,7 +638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="138" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -678,7 +655,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="92" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -695,7 +672,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="207" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -712,154 +689,160 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="253" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7">
         <v>43210</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="23" x14ac:dyDescent="0.4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7">
+        <v>43215</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="23" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="23" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -872,12 +855,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -885,12 +868,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>